<commit_message>
start process of adding games
</commit_message>
<xml_diff>
--- a/ranges.xlsx
+++ b/ranges.xlsx
@@ -1,26 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\FCFB-Ref-Bot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apkick/Documents/Programming/Spyder/FakeCFBRefBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE260B9-3E2F-4916-9FF9-5C6E1AB0C5CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Ranges" sheetId="1" r:id="rId1"/>
+    <sheet name="Kickoff and PAT" sheetId="2" r:id="rId2"/>
+    <sheet name="Punt" sheetId="3" r:id="rId3"/>
+    <sheet name="Field Goal" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -3143,8 +3148,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3938,6 +3943,15 @@
     <xf numFmtId="16" fontId="8" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3946,15 +3960,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4244,16 +4249,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AE21" sqref="AE21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:54" ht="15.75" thickBot="1">
+    <row r="1" spans="1:54" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -4309,7 +4314,7 @@
       <c r="AY1" s="5"/>
       <c r="AZ1" s="5"/>
     </row>
-    <row r="2" spans="1:54" ht="15.75" thickBot="1">
+    <row r="2" spans="1:54" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -4467,7 +4472,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="15.75" thickBot="1">
+    <row r="3" spans="1:54" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -4623,7 +4628,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:54" ht="15.75" thickBot="1">
+    <row r="4" spans="1:54" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
@@ -4781,7 +4786,7 @@
       <c r="BA4" s="32"/>
       <c r="BB4" s="32"/>
     </row>
-    <row r="5" spans="1:54" ht="26.25" thickBot="1">
+    <row r="5" spans="1:54" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
@@ -4842,7 +4847,7 @@
       <c r="AZ5" s="36"/>
       <c r="BA5" s="32"/>
     </row>
-    <row r="6" spans="1:54" ht="26.25" thickBot="1">
+    <row r="6" spans="1:54" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>14</v>
       </c>
@@ -5000,7 +5005,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:54" ht="26.25" thickBot="1">
+    <row r="7" spans="1:54" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>16</v>
       </c>
@@ -5158,7 +5163,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="8" spans="1:54" ht="26.25" thickBot="1">
+    <row r="8" spans="1:54" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>17</v>
       </c>
@@ -5316,7 +5321,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="9" spans="1:54" ht="26.25" thickBot="1">
+    <row r="9" spans="1:54" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>18</v>
       </c>
@@ -5474,7 +5479,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="10" spans="1:54" ht="26.25" thickBot="1">
+    <row r="10" spans="1:54" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>19</v>
       </c>
@@ -5632,7 +5637,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:54" ht="15.75" thickBot="1">
+    <row r="11" spans="1:54" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>21</v>
       </c>
@@ -5790,7 +5795,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:54" ht="26.25" thickBot="1">
+    <row r="12" spans="1:54" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>23</v>
       </c>
@@ -5948,7 +5953,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:54" ht="26.25" thickBot="1">
+    <row r="13" spans="1:54" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>25</v>
       </c>
@@ -6106,7 +6111,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="14" spans="1:54" ht="26.25" thickBot="1">
+    <row r="14" spans="1:54" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>26</v>
       </c>
@@ -6264,7 +6269,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="15" spans="1:54" ht="26.25" thickBot="1">
+    <row r="15" spans="1:54" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>27</v>
       </c>
@@ -6422,7 +6427,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="16" spans="1:54" ht="15.75" thickBot="1">
+    <row r="16" spans="1:54" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>-10</v>
       </c>
@@ -6580,7 +6585,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:52" ht="15.75" thickBot="1">
+    <row r="17" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>-5</v>
       </c>
@@ -6738,7 +6743,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:52" ht="15.75" thickBot="1">
+    <row r="18" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>-3</v>
       </c>
@@ -6896,7 +6901,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:52" ht="15.75" thickBot="1">
+    <row r="19" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>-1</v>
       </c>
@@ -7054,7 +7059,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:52" ht="15.75" thickBot="1">
+    <row r="20" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>51</v>
       </c>
@@ -7212,7 +7217,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:52" ht="26.25" thickBot="1">
+    <row r="21" spans="1:52" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>77</v>
       </c>
@@ -7370,7 +7375,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="22" spans="1:52" ht="15.75" thickBot="1">
+    <row r="22" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>1</v>
       </c>
@@ -7528,7 +7533,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="23" spans="1:52" ht="15.75" thickBot="1">
+    <row r="23" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>2</v>
       </c>
@@ -7686,7 +7691,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="1:52" ht="15.75" thickBot="1">
+    <row r="24" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>3</v>
       </c>
@@ -7844,7 +7849,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="25" spans="1:52" ht="15.75" thickBot="1">
+    <row r="25" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>4</v>
       </c>
@@ -8002,7 +8007,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="26" spans="1:52" ht="15.75" thickBot="1">
+    <row r="26" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>5</v>
       </c>
@@ -8160,7 +8165,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="27" spans="1:52" ht="15.75" thickBot="1">
+    <row r="27" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>6</v>
       </c>
@@ -8318,7 +8323,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="28" spans="1:52" ht="15.75" thickBot="1">
+    <row r="28" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>7</v>
       </c>
@@ -8476,7 +8481,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="29" spans="1:52" ht="15.75" thickBot="1">
+    <row r="29" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>8</v>
       </c>
@@ -8634,7 +8639,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="30" spans="1:52" ht="15.75" thickBot="1">
+    <row r="30" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>9</v>
       </c>
@@ -8792,7 +8797,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="31" spans="1:52" ht="15.75" thickBot="1">
+    <row r="31" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>10</v>
       </c>
@@ -8950,7 +8955,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="32" spans="1:52" ht="15.75" thickBot="1">
+    <row r="32" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>11</v>
       </c>
@@ -9108,7 +9113,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="33" spans="1:52" ht="15.75" thickBot="1">
+    <row r="33" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>12</v>
       </c>
@@ -9266,7 +9271,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="34" spans="1:52" ht="15.75" thickBot="1">
+    <row r="34" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>13</v>
       </c>
@@ -9424,7 +9429,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="35" spans="1:52" ht="15.75" thickBot="1">
+    <row r="35" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>14</v>
       </c>
@@ -9582,7 +9587,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="36" spans="1:52" ht="15.75" thickBot="1">
+    <row r="36" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <v>15</v>
       </c>
@@ -9740,7 +9745,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="37" spans="1:52" ht="15.75" thickBot="1">
+    <row r="37" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <v>16</v>
       </c>
@@ -9898,7 +9903,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="38" spans="1:52" ht="15.75" thickBot="1">
+    <row r="38" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>17</v>
       </c>
@@ -10056,7 +10061,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="39" spans="1:52" ht="15.75" thickBot="1">
+    <row r="39" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <v>18</v>
       </c>
@@ -10214,7 +10219,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="40" spans="1:52" ht="15.75" thickBot="1">
+    <row r="40" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <v>19</v>
       </c>
@@ -10372,7 +10377,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="41" spans="1:52" ht="15.75" thickBot="1">
+    <row r="41" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <v>20</v>
       </c>
@@ -10530,7 +10535,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="42" spans="1:52" ht="15.75" thickBot="1">
+    <row r="42" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <v>25</v>
       </c>
@@ -10688,7 +10693,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="43" spans="1:52" ht="15.75" thickBot="1">
+    <row r="43" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
         <v>30</v>
       </c>
@@ -10846,7 +10851,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="44" spans="1:52" ht="15.75" thickBot="1">
+    <row r="44" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <v>35</v>
       </c>
@@ -11004,7 +11009,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="45" spans="1:52" ht="15.75" thickBot="1">
+    <row r="45" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <v>40</v>
       </c>
@@ -11162,7 +11167,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="46" spans="1:52" ht="15.75" thickBot="1">
+    <row r="46" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <v>45</v>
       </c>
@@ -11320,7 +11325,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="47" spans="1:52" ht="15.75" thickBot="1">
+    <row r="47" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
         <v>50</v>
       </c>
@@ -11478,7 +11483,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="48" spans="1:52" ht="15.75" thickBot="1">
+    <row r="48" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
         <v>55</v>
       </c>
@@ -11636,7 +11641,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="49" spans="1:52" ht="15.75" thickBot="1">
+    <row r="49" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
         <v>60</v>
       </c>
@@ -11794,7 +11799,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="50" spans="1:52" ht="15.75" thickBot="1">
+    <row r="50" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12">
         <v>65</v>
       </c>
@@ -11952,7 +11957,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="51" spans="1:52" ht="15.75" thickBot="1">
+    <row r="51" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12">
         <v>70</v>
       </c>
@@ -12110,7 +12115,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="52" spans="1:52" ht="15.75" thickBot="1">
+    <row r="52" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12">
         <v>75</v>
       </c>
@@ -12268,7 +12273,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="53" spans="1:52" ht="15.75" thickBot="1">
+    <row r="53" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="12">
         <v>80</v>
       </c>
@@ -12426,7 +12431,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="54" spans="1:52" ht="15.75" thickBot="1">
+    <row r="54" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="12">
         <v>85</v>
       </c>
@@ -12584,7 +12589,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="55" spans="1:52" ht="15.75" thickBot="1">
+    <row r="55" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="12">
         <v>90</v>
       </c>
@@ -12742,7 +12747,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="56" spans="1:52" ht="15.75" thickBot="1">
+    <row r="56" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="12">
         <v>95</v>
       </c>
@@ -12900,7 +12905,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="57" spans="1:52" ht="26.25" thickBot="1">
+    <row r="57" spans="1:52" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="21" t="s">
         <v>850</v>
       </c>
@@ -13058,7 +13063,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="58" spans="1:52" ht="15.75" thickBot="1">
+    <row r="58" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="23" t="s">
         <v>852</v>
       </c>
@@ -13214,7 +13219,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:52" ht="15.75" thickBot="1">
+    <row r="59" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="26" t="s">
         <v>853</v>
       </c>
@@ -13278,16 +13283,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{123F6202-B349-430D-BFCA-ACEC89327060}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" thickBot="1">
+    <row r="1" spans="1:9" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
         <v>861</v>
       </c>
@@ -13300,7 +13305,7 @@
       <c r="H1" s="43"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1">
+    <row r="2" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="44"/>
       <c r="B2" s="45" t="s">
         <v>862</v>
@@ -13315,7 +13320,7 @@
       <c r="H2" s="45"/>
       <c r="I2" s="45"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1">
+    <row r="3" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
         <v>864</v>
       </c>
@@ -13334,7 +13339,7 @@
       <c r="H3" s="45"/>
       <c r="I3" s="45"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1">
+    <row r="4" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
         <v>867</v>
       </c>
@@ -13353,7 +13358,7 @@
       <c r="H4" s="45"/>
       <c r="I4" s="45"/>
     </row>
-    <row r="5" spans="1:9" ht="27" thickBot="1">
+    <row r="5" spans="1:9" ht="28" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="s">
         <v>870</v>
       </c>
@@ -13372,7 +13377,7 @@
       <c r="H5" s="45"/>
       <c r="I5" s="45"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1">
+    <row r="6" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="44"/>
       <c r="B6" s="45"/>
       <c r="C6" s="45"/>
@@ -13383,7 +13388,7 @@
       <c r="H6" s="45"/>
       <c r="I6" s="45"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1">
+    <row r="7" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="44"/>
       <c r="B7" s="45" t="s">
         <v>871</v>
@@ -13406,7 +13411,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="27" thickBot="1">
+    <row r="8" spans="1:9" ht="28" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
         <v>850</v>
       </c>
@@ -13435,7 +13440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1">
+    <row r="9" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="46" t="s">
         <v>876</v>
       </c>
@@ -13464,7 +13469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="27" thickBot="1">
+    <row r="10" spans="1:9" ht="28" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="46">
         <v>10</v>
       </c>
@@ -13493,7 +13498,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1">
+    <row r="11" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="44">
         <v>20</v>
       </c>
@@ -13516,7 +13521,7 @@
       <c r="H11" s="45"/>
       <c r="I11" s="45"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1">
+    <row r="12" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="46">
         <v>25</v>
       </c>
@@ -13539,7 +13544,7 @@
       <c r="H12" s="45"/>
       <c r="I12" s="45"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1">
+    <row r="13" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="46">
         <v>30</v>
       </c>
@@ -13562,7 +13567,7 @@
       <c r="H13" s="45"/>
       <c r="I13" s="45"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1">
+    <row r="14" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="46">
         <v>40</v>
       </c>
@@ -13585,7 +13590,7 @@
       <c r="H14" s="45"/>
       <c r="I14" s="45"/>
     </row>
-    <row r="15" spans="1:9" ht="26.25" thickBot="1">
+    <row r="15" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="44">
         <v>50</v>
       </c>
@@ -13608,7 +13613,7 @@
       <c r="H15" s="45"/>
       <c r="I15" s="45"/>
     </row>
-    <row r="16" spans="1:9" ht="26.25" thickBot="1">
+    <row r="16" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
         <v>880</v>
       </c>
@@ -13632,16 +13637,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12713F6F-10AB-4DF5-96AA-717BFA09BC2D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:O22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="47.25" thickBot="1">
+    <row r="1" spans="1:15" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>890</v>
       </c>
@@ -13662,7 +13667,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="26.25" thickBot="1">
+    <row r="2" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>892</v>
       </c>
@@ -13709,28 +13714,28 @@
         <v>36647</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="26.25" thickBot="1">
+    <row r="3" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="63"/>
-      <c r="O3" s="64"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="66"/>
+      <c r="N3" s="66"/>
+      <c r="O3" s="67"/>
     </row>
-    <row r="4" spans="1:15" ht="15.75" thickBot="1">
+    <row r="4" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>905</v>
       </c>
@@ -13777,7 +13782,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" thickBot="1">
+    <row r="5" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>907</v>
       </c>
@@ -13824,7 +13829,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" thickBot="1">
+    <row r="6" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -13869,7 +13874,7 @@
       </c>
       <c r="O6" s="47"/>
     </row>
-    <row r="7" spans="1:15" ht="15.75" thickBot="1">
+    <row r="7" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>10</v>
       </c>
@@ -13912,7 +13917,7 @@
       <c r="N7" s="47"/>
       <c r="O7" s="47"/>
     </row>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1">
+    <row r="8" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>15</v>
       </c>
@@ -13939,7 +13944,7 @@
       <c r="N8" s="47"/>
       <c r="O8" s="47"/>
     </row>
-    <row r="9" spans="1:15" ht="15.75" thickBot="1">
+    <row r="9" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>20</v>
       </c>
@@ -13966,7 +13971,7 @@
       <c r="N9" s="47"/>
       <c r="O9" s="47"/>
     </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1">
+    <row r="10" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>25</v>
       </c>
@@ -14003,7 +14008,7 @@
       <c r="N10" s="47"/>
       <c r="O10" s="47"/>
     </row>
-    <row r="11" spans="1:15" ht="15.75" thickBot="1">
+    <row r="11" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>30</v>
       </c>
@@ -14030,7 +14035,7 @@
       <c r="N11" s="47"/>
       <c r="O11" s="47"/>
     </row>
-    <row r="12" spans="1:15" ht="15.75" thickBot="1">
+    <row r="12" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>35</v>
       </c>
@@ -14063,7 +14068,7 @@
       <c r="N12" s="47"/>
       <c r="O12" s="47"/>
     </row>
-    <row r="13" spans="1:15" ht="15.75" thickBot="1">
+    <row r="13" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>40</v>
       </c>
@@ -14094,7 +14099,7 @@
       <c r="N13" s="47"/>
       <c r="O13" s="47"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" thickBot="1">
+    <row r="14" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>45</v>
       </c>
@@ -14123,7 +14128,7 @@
       <c r="N14" s="47"/>
       <c r="O14" s="47"/>
     </row>
-    <row r="15" spans="1:15" ht="15.75" thickBot="1">
+    <row r="15" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>50</v>
       </c>
@@ -14150,7 +14155,7 @@
       <c r="N15" s="47"/>
       <c r="O15" s="47"/>
     </row>
-    <row r="16" spans="1:15" ht="15.75" thickBot="1">
+    <row r="16" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>55</v>
       </c>
@@ -14175,7 +14180,7 @@
       <c r="N16" s="47"/>
       <c r="O16" s="47"/>
     </row>
-    <row r="17" spans="1:15" ht="15.75" thickBot="1">
+    <row r="17" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>60</v>
       </c>
@@ -14198,7 +14203,7 @@
       <c r="N17" s="47"/>
       <c r="O17" s="47"/>
     </row>
-    <row r="18" spans="1:15" ht="15.75" thickBot="1">
+    <row r="18" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>65</v>
       </c>
@@ -14219,7 +14224,7 @@
       <c r="N18" s="47"/>
       <c r="O18" s="47"/>
     </row>
-    <row r="19" spans="1:15" ht="26.25" thickBot="1">
+    <row r="19" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>919</v>
       </c>
@@ -14264,7 +14269,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15.75" thickBot="1">
+    <row r="20" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>876</v>
       </c>
@@ -14311,7 +14316,7 @@
         <v>43854</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="26.25" thickBot="1">
+    <row r="21" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>850</v>
       </c>
@@ -14358,7 +14363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15.75" thickBot="1">
+    <row r="22" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
         <v>3</v>
       </c>
@@ -14388,16 +14393,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BA07ED-E1FF-4201-AF75-CF1B776C7687}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="24" thickBot="1">
+    <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="68" t="s">
         <v>930</v>
       </c>
@@ -14406,7 +14411,7 @@
       <c r="D1" s="69"/>
       <c r="E1" s="70"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1">
+    <row r="2" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>931</v>
       </c>
@@ -14423,18 +14428,18 @@
         <v>934</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="26.25" thickBot="1">
+    <row r="3" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="64"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="67"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1">
+    <row r="4" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>17</v>
       </c>
@@ -14445,11 +14450,11 @@
       <c r="D4" s="47" t="s">
         <v>936</v>
       </c>
-      <c r="E4" s="65" t="s">
+      <c r="E4" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1">
+    <row r="5" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="46">
         <v>18</v>
       </c>
@@ -14460,11 +14465,11 @@
       <c r="D5" s="47" t="s">
         <v>939</v>
       </c>
-      <c r="E5" s="65" t="s">
+      <c r="E5" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1">
+    <row r="6" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="46">
         <v>19</v>
       </c>
@@ -14475,11 +14480,11 @@
       <c r="D6" s="47" t="s">
         <v>941</v>
       </c>
-      <c r="E6" s="65" t="s">
+      <c r="E6" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1">
+    <row r="7" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="46">
         <v>20</v>
       </c>
@@ -14490,11 +14495,11 @@
       <c r="D7" s="47" t="s">
         <v>943</v>
       </c>
-      <c r="E7" s="65" t="s">
+      <c r="E7" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1">
+    <row r="8" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>21</v>
       </c>
@@ -14505,11 +14510,11 @@
       <c r="D8" s="47" t="s">
         <v>945</v>
       </c>
-      <c r="E8" s="65" t="s">
+      <c r="E8" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1">
+    <row r="9" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="46">
         <v>22</v>
       </c>
@@ -14520,11 +14525,11 @@
       <c r="D9" s="47" t="s">
         <v>947</v>
       </c>
-      <c r="E9" s="65" t="s">
+      <c r="E9" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1">
+    <row r="10" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="46">
         <v>23</v>
       </c>
@@ -14537,11 +14542,11 @@
       <c r="D10" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E10" s="65" t="s">
+      <c r="E10" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1">
+    <row r="11" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="46">
         <v>24</v>
       </c>
@@ -14554,11 +14559,11 @@
       <c r="D11" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E11" s="65" t="s">
+      <c r="E11" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1">
+    <row r="12" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>25</v>
       </c>
@@ -14571,11 +14576,11 @@
       <c r="D12" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E12" s="65" t="s">
+      <c r="E12" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1">
+    <row r="13" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="46">
         <v>26</v>
       </c>
@@ -14588,11 +14593,11 @@
       <c r="D13" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E13" s="65" t="s">
+      <c r="E13" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1">
+    <row r="14" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="46">
         <v>27</v>
       </c>
@@ -14605,11 +14610,11 @@
       <c r="D14" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E14" s="65" t="s">
+      <c r="E14" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1">
+    <row r="15" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="46">
         <v>28</v>
       </c>
@@ -14622,11 +14627,11 @@
       <c r="D15" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E15" s="65" t="s">
+      <c r="E15" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1">
+    <row r="16" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>29</v>
       </c>
@@ -14639,11 +14644,11 @@
       <c r="D16" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E16" s="65" t="s">
+      <c r="E16" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1">
+    <row r="17" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>30</v>
       </c>
@@ -14656,11 +14661,11 @@
       <c r="D17" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E17" s="65" t="s">
+      <c r="E17" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1">
+    <row r="18" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="46">
         <v>31</v>
       </c>
@@ -14673,11 +14678,11 @@
       <c r="D18" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E18" s="65" t="s">
+      <c r="E18" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1">
+    <row r="19" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="46">
         <v>32</v>
       </c>
@@ -14690,11 +14695,11 @@
       <c r="D19" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E19" s="65" t="s">
+      <c r="E19" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1">
+    <row r="20" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="46">
         <v>33</v>
       </c>
@@ -14707,11 +14712,11 @@
       <c r="D20" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E20" s="65" t="s">
+      <c r="E20" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1">
+    <row r="21" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>34</v>
       </c>
@@ -14724,11 +14729,11 @@
       <c r="D21" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E21" s="65" t="s">
+      <c r="E21" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1">
+    <row r="22" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="46">
         <v>35</v>
       </c>
@@ -14741,11 +14746,11 @@
       <c r="D22" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E22" s="65" t="s">
+      <c r="E22" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1">
+    <row r="23" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="46">
         <v>36</v>
       </c>
@@ -14758,11 +14763,11 @@
       <c r="D23" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E23" s="65" t="s">
+      <c r="E23" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1">
+    <row r="24" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="46">
         <v>37</v>
       </c>
@@ -14775,11 +14780,11 @@
       <c r="D24" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E24" s="65" t="s">
+      <c r="E24" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1">
+    <row r="25" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>38</v>
       </c>
@@ -14792,11 +14797,11 @@
       <c r="D25" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E25" s="65" t="s">
+      <c r="E25" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1">
+    <row r="26" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="46">
         <v>39</v>
       </c>
@@ -14809,11 +14814,11 @@
       <c r="D26" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E26" s="65" t="s">
+      <c r="E26" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1">
+    <row r="27" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="46">
         <v>40</v>
       </c>
@@ -14826,11 +14831,11 @@
       <c r="D27" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E27" s="65" t="s">
+      <c r="E27" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1">
+    <row r="28" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="46">
         <v>41</v>
       </c>
@@ -14843,11 +14848,11 @@
       <c r="D28" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E28" s="65" t="s">
+      <c r="E28" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1">
+    <row r="29" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>42</v>
       </c>
@@ -14860,11 +14865,11 @@
       <c r="D29" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E29" s="65" t="s">
+      <c r="E29" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1">
+    <row r="30" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>43</v>
       </c>
@@ -14877,11 +14882,11 @@
       <c r="D30" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E30" s="65" t="s">
+      <c r="E30" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1">
+    <row r="31" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="46">
         <v>44</v>
       </c>
@@ -14894,11 +14899,11 @@
       <c r="D31" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E31" s="65" t="s">
+      <c r="E31" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1">
+    <row r="32" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="46">
         <v>45</v>
       </c>
@@ -14911,11 +14916,11 @@
       <c r="D32" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E32" s="65" t="s">
+      <c r="E32" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" thickBot="1">
+    <row r="33" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="46">
         <v>46</v>
       </c>
@@ -14928,11 +14933,11 @@
       <c r="D33" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E33" s="65" t="s">
+      <c r="E33" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" thickBot="1">
+    <row r="34" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>47</v>
       </c>
@@ -14945,11 +14950,11 @@
       <c r="D34" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E34" s="65" t="s">
+      <c r="E34" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" thickBot="1">
+    <row r="35" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="46">
         <v>48</v>
       </c>
@@ -14962,11 +14967,11 @@
       <c r="D35" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E35" s="65" t="s">
+      <c r="E35" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" thickBot="1">
+    <row r="36" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="46">
         <v>49</v>
       </c>
@@ -14979,11 +14984,11 @@
       <c r="D36" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E36" s="65" t="s">
+      <c r="E36" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" thickBot="1">
+    <row r="37" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="46">
         <v>50</v>
       </c>
@@ -14996,11 +15001,11 @@
       <c r="D37" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E37" s="65" t="s">
+      <c r="E37" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" thickBot="1">
+    <row r="38" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>51</v>
       </c>
@@ -15013,11 +15018,11 @@
       <c r="D38" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E38" s="65" t="s">
+      <c r="E38" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" thickBot="1">
+    <row r="39" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>52</v>
       </c>
@@ -15030,11 +15035,11 @@
       <c r="D39" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E39" s="65" t="s">
+      <c r="E39" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" thickBot="1">
+    <row r="40" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="46">
         <v>53</v>
       </c>
@@ -15047,11 +15052,11 @@
       <c r="D40" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E40" s="65" t="s">
+      <c r="E40" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" thickBot="1">
+    <row r="41" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="46">
         <v>54</v>
       </c>
@@ -15064,11 +15069,11 @@
       <c r="D41" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E41" s="65" t="s">
+      <c r="E41" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" thickBot="1">
+    <row r="42" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="46">
         <v>55</v>
       </c>
@@ -15081,11 +15086,11 @@
       <c r="D42" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E42" s="65" t="s">
+      <c r="E42" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" thickBot="1">
+    <row r="43" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>56</v>
       </c>
@@ -15098,11 +15103,11 @@
       <c r="D43" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E43" s="65" t="s">
+      <c r="E43" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" thickBot="1">
+    <row r="44" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="46">
         <v>57</v>
       </c>
@@ -15115,15 +15120,15 @@
       <c r="D44" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E44" s="65" t="s">
+      <c r="E44" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" thickBot="1">
+    <row r="45" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="46">
         <v>58</v>
       </c>
-      <c r="B45" s="66" t="s">
+      <c r="B45" s="63" t="s">
         <v>1019</v>
       </c>
       <c r="C45" s="47" t="s">
@@ -15132,15 +15137,15 @@
       <c r="D45" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E45" s="65" t="s">
+      <c r="E45" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" thickBot="1">
+    <row r="46" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="46">
         <v>59</v>
       </c>
-      <c r="B46" s="66" t="s">
+      <c r="B46" s="63" t="s">
         <v>1021</v>
       </c>
       <c r="C46" s="47" t="s">
@@ -15149,15 +15154,15 @@
       <c r="D46" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E46" s="65" t="s">
+      <c r="E46" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" thickBot="1">
+    <row r="47" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="46">
         <v>60</v>
       </c>
-      <c r="B47" s="66" t="s">
+      <c r="B47" s="63" t="s">
         <v>1023</v>
       </c>
       <c r="C47" s="47" t="s">
@@ -15166,15 +15171,15 @@
       <c r="D47" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E47" s="65" t="s">
+      <c r="E47" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" thickBot="1">
+    <row r="48" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="46">
         <v>61</v>
       </c>
-      <c r="B48" s="66" t="s">
+      <c r="B48" s="63" t="s">
         <v>1025</v>
       </c>
       <c r="C48" s="47" t="s">
@@ -15183,15 +15188,15 @@
       <c r="D48" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E48" s="65" t="s">
+      <c r="E48" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15.75" thickBot="1">
+    <row r="49" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="46">
         <v>62</v>
       </c>
-      <c r="B49" s="66" t="s">
+      <c r="B49" s="63" t="s">
         <v>1027</v>
       </c>
       <c r="C49" s="47" t="s">
@@ -15200,15 +15205,15 @@
       <c r="D49" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E49" s="65" t="s">
+      <c r="E49" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15.75" thickBot="1">
+    <row r="50" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="46">
         <v>63</v>
       </c>
-      <c r="B50" s="66" t="s">
+      <c r="B50" s="63" t="s">
         <v>1029</v>
       </c>
       <c r="C50" s="47" t="s">
@@ -15217,15 +15222,15 @@
       <c r="D50" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E50" s="65" t="s">
+      <c r="E50" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15.75" thickBot="1">
+    <row r="51" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="46">
         <v>64</v>
       </c>
-      <c r="B51" s="66" t="s">
+      <c r="B51" s="63" t="s">
         <v>1031</v>
       </c>
       <c r="C51" s="47" t="s">
@@ -15234,15 +15239,15 @@
       <c r="D51" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E51" s="65" t="s">
+      <c r="E51" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15.75" thickBot="1">
+    <row r="52" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="46">
         <v>65</v>
       </c>
-      <c r="B52" s="66">
+      <c r="B52" s="63">
         <v>0</v>
       </c>
       <c r="C52" s="47" t="s">
@@ -15251,11 +15256,11 @@
       <c r="D52" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E52" s="65" t="s">
+      <c r="E52" s="62" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15.75" thickBot="1">
+    <row r="53" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="26" t="s">
         <v>3</v>
       </c>
@@ -15266,7 +15271,7 @@
       <c r="D53" s="30">
         <v>5</v>
       </c>
-      <c r="E53" s="67">
+      <c r="E53" s="64">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
get coin toss working and start on kickoff
</commit_message>
<xml_diff>
--- a/ranges.xlsx
+++ b/ranges.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apkick/Documents/Programming/Spyder/FakeCFBRefBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6F4A68-23A9-7B4E-B3A9-7A54F5A73F4C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ranges" sheetId="1" r:id="rId1"/>
@@ -22,18 +23,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2856" uniqueCount="1034">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2858" uniqueCount="1035">
   <si>
     <t>FakeCFB Ranges by UVA</t>
   </si>
@@ -3144,11 +3145,14 @@
   <si>
     <t>1-700</t>
   </si>
+  <si>
+    <t>1-15</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3168,40 +3172,47 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFD9D9D9"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -3910,9 +3921,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3968,6 +3976,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4249,7 +4260,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4786,7 +4797,7 @@
       <c r="BA4" s="32"/>
       <c r="BB4" s="32"/>
     </row>
-    <row r="5" spans="1:54" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
@@ -4847,7 +4858,7 @@
       <c r="AZ5" s="36"/>
       <c r="BA5" s="32"/>
     </row>
-    <row r="6" spans="1:54" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>14</v>
       </c>
@@ -5005,7 +5016,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:54" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>16</v>
       </c>
@@ -5163,7 +5174,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="8" spans="1:54" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>17</v>
       </c>
@@ -5321,7 +5332,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="9" spans="1:54" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>18</v>
       </c>
@@ -5479,7 +5490,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="10" spans="1:54" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>19</v>
       </c>
@@ -5795,7 +5806,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:54" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>23</v>
       </c>
@@ -5953,7 +5964,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:54" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>25</v>
       </c>
@@ -6111,7 +6122,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="14" spans="1:54" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>26</v>
       </c>
@@ -6269,7 +6280,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="15" spans="1:54" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>27</v>
       </c>
@@ -7217,7 +7228,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:52" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:52" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>77</v>
       </c>
@@ -12905,7 +12916,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="57" spans="1:52" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:52" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="21" t="s">
         <v>850</v>
       </c>
@@ -13283,11 +13294,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13358,7 +13369,7 @@
       <c r="H4" s="45"/>
       <c r="I4" s="45"/>
     </row>
-    <row r="5" spans="1:9" ht="28" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="30" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="s">
         <v>870</v>
       </c>
@@ -13411,7 +13422,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="28" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="30" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
         <v>850</v>
       </c>
@@ -13444,8 +13455,8 @@
       <c r="A9" s="46" t="s">
         <v>876</v>
       </c>
-      <c r="B9" s="51">
-        <v>43845</v>
+      <c r="B9" s="70" t="s">
+        <v>1034</v>
       </c>
       <c r="C9" s="50">
         <v>5</v>
@@ -13453,8 +13464,8 @@
       <c r="D9" s="48" t="s">
         <v>876</v>
       </c>
-      <c r="E9" s="51">
-        <v>43845</v>
+      <c r="E9" s="70" t="s">
+        <v>1034</v>
       </c>
       <c r="F9" s="50">
         <v>3</v>
@@ -13465,11 +13476,11 @@
       <c r="H9" s="47" t="s">
         <v>877</v>
       </c>
-      <c r="I9" s="52">
+      <c r="I9" s="51">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="28" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="30" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="46">
         <v>10</v>
       </c>
@@ -13494,7 +13505,7 @@
       <c r="H10" s="47">
         <v>750</v>
       </c>
-      <c r="I10" s="52">
+      <c r="I10" s="51">
         <v>10</v>
       </c>
     </row>
@@ -13590,7 +13601,7 @@
       <c r="H14" s="45"/>
       <c r="I14" s="45"/>
     </row>
-    <row r="15" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="44">
         <v>50</v>
       </c>
@@ -13606,21 +13617,21 @@
       <c r="E15" s="47" t="s">
         <v>888</v>
       </c>
-      <c r="F15" s="52">
+      <c r="F15" s="51">
         <v>13</v>
       </c>
       <c r="G15" s="45"/>
       <c r="H15" s="45"/>
       <c r="I15" s="45"/>
     </row>
-    <row r="16" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
         <v>880</v>
       </c>
       <c r="B16" s="47" t="s">
         <v>889</v>
       </c>
-      <c r="C16" s="52">
+      <c r="C16" s="51">
         <v>13</v>
       </c>
       <c r="D16" s="45"/>
@@ -13637,7 +13648,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13646,28 +13657,28 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="24" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:15" ht="25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
         <v>890</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="56" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="55" t="s">
         <v>891</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>892</v>
       </c>
@@ -13710,75 +13721,75 @@
       <c r="N2" s="10">
         <v>44110</v>
       </c>
-      <c r="O2" s="57">
+      <c r="O2" s="56">
         <v>36647</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
-      <c r="N3" s="66"/>
-      <c r="O3" s="67"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="65"/>
+      <c r="O3" s="66"/>
     </row>
     <row r="4" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>905</v>
       </c>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="57" t="s">
         <v>906</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="57" t="s">
         <v>906</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="57" t="s">
         <v>906</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="E4" s="57" t="s">
         <v>906</v>
       </c>
-      <c r="F4" s="58" t="s">
+      <c r="F4" s="57" t="s">
         <v>906</v>
       </c>
-      <c r="G4" s="58" t="s">
+      <c r="G4" s="57" t="s">
         <v>906</v>
       </c>
-      <c r="H4" s="58" t="s">
+      <c r="H4" s="57" t="s">
         <v>906</v>
       </c>
-      <c r="I4" s="58" t="s">
+      <c r="I4" s="57" t="s">
         <v>906</v>
       </c>
-      <c r="J4" s="58" t="s">
+      <c r="J4" s="57" t="s">
         <v>906</v>
       </c>
-      <c r="K4" s="58" t="s">
+      <c r="K4" s="57" t="s">
         <v>906</v>
       </c>
-      <c r="L4" s="58" t="s">
+      <c r="L4" s="57" t="s">
         <v>906</v>
       </c>
-      <c r="M4" s="58" t="s">
+      <c r="M4" s="57" t="s">
         <v>906</v>
       </c>
-      <c r="N4" s="58" t="s">
+      <c r="N4" s="57" t="s">
         <v>906</v>
       </c>
-      <c r="O4" s="58" t="s">
+      <c r="O4" s="57" t="s">
         <v>906</v>
       </c>
     </row>
@@ -13786,46 +13797,46 @@
       <c r="A5" s="6" t="s">
         <v>907</v>
       </c>
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="57" t="s">
         <v>908</v>
       </c>
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="57" t="s">
         <v>908</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="D5" s="57" t="s">
         <v>908</v>
       </c>
-      <c r="E5" s="58" t="s">
+      <c r="E5" s="57" t="s">
         <v>908</v>
       </c>
-      <c r="F5" s="58" t="s">
+      <c r="F5" s="57" t="s">
         <v>908</v>
       </c>
-      <c r="G5" s="58" t="s">
+      <c r="G5" s="57" t="s">
         <v>908</v>
       </c>
-      <c r="H5" s="58" t="s">
+      <c r="H5" s="57" t="s">
         <v>908</v>
       </c>
-      <c r="I5" s="58" t="s">
+      <c r="I5" s="57" t="s">
         <v>908</v>
       </c>
-      <c r="J5" s="58" t="s">
+      <c r="J5" s="57" t="s">
         <v>908</v>
       </c>
-      <c r="K5" s="58" t="s">
+      <c r="K5" s="57" t="s">
         <v>908</v>
       </c>
-      <c r="L5" s="58" t="s">
+      <c r="L5" s="57" t="s">
         <v>908</v>
       </c>
-      <c r="M5" s="58" t="s">
+      <c r="M5" s="57" t="s">
         <v>908</v>
       </c>
-      <c r="N5" s="58" t="s">
+      <c r="N5" s="57" t="s">
         <v>908</v>
       </c>
-      <c r="O5" s="58" t="s">
+      <c r="O5" s="57" t="s">
         <v>908</v>
       </c>
     </row>
@@ -13860,16 +13871,16 @@
       <c r="J6" s="47" t="s">
         <v>909</v>
       </c>
-      <c r="K6" s="59" t="s">
+      <c r="K6" s="58" t="s">
         <v>910</v>
       </c>
-      <c r="L6" s="59" t="s">
+      <c r="L6" s="58" t="s">
         <v>911</v>
       </c>
-      <c r="M6" s="59" t="s">
+      <c r="M6" s="58" t="s">
         <v>912</v>
       </c>
-      <c r="N6" s="59" t="s">
+      <c r="N6" s="58" t="s">
         <v>913</v>
       </c>
       <c r="O6" s="47"/>
@@ -13902,16 +13913,16 @@
       <c r="I7" s="47" t="s">
         <v>914</v>
       </c>
-      <c r="J7" s="59" t="s">
+      <c r="J7" s="58" t="s">
         <v>910</v>
       </c>
-      <c r="K7" s="59" t="s">
+      <c r="K7" s="58" t="s">
         <v>911</v>
       </c>
-      <c r="L7" s="59" t="s">
+      <c r="L7" s="58" t="s">
         <v>912</v>
       </c>
-      <c r="M7" s="59" t="s">
+      <c r="M7" s="58" t="s">
         <v>913</v>
       </c>
       <c r="N7" s="47"/>
@@ -13928,16 +13939,16 @@
       <c r="F8" s="47"/>
       <c r="G8" s="47"/>
       <c r="H8" s="47"/>
-      <c r="I8" s="59" t="s">
+      <c r="I8" s="58" t="s">
         <v>910</v>
       </c>
-      <c r="J8" s="59" t="s">
+      <c r="J8" s="58" t="s">
         <v>911</v>
       </c>
-      <c r="K8" s="59" t="s">
+      <c r="K8" s="58" t="s">
         <v>912</v>
       </c>
-      <c r="L8" s="59" t="s">
+      <c r="L8" s="58" t="s">
         <v>913</v>
       </c>
       <c r="M8" s="47"/>
@@ -13954,16 +13965,16 @@
       <c r="E9" s="47"/>
       <c r="F9" s="47"/>
       <c r="G9" s="47"/>
-      <c r="H9" s="59" t="s">
+      <c r="H9" s="58" t="s">
         <v>910</v>
       </c>
-      <c r="I9" s="59" t="s">
+      <c r="I9" s="58" t="s">
         <v>911</v>
       </c>
-      <c r="J9" s="59" t="s">
+      <c r="J9" s="58" t="s">
         <v>912</v>
       </c>
-      <c r="K9" s="59" t="s">
+      <c r="K9" s="58" t="s">
         <v>913</v>
       </c>
       <c r="L9" s="47"/>
@@ -13990,16 +14001,16 @@
       <c r="F10" s="47" t="s">
         <v>915</v>
       </c>
-      <c r="G10" s="59" t="s">
+      <c r="G10" s="58" t="s">
         <v>910</v>
       </c>
-      <c r="H10" s="59" t="s">
+      <c r="H10" s="58" t="s">
         <v>911</v>
       </c>
-      <c r="I10" s="59" t="s">
+      <c r="I10" s="58" t="s">
         <v>912</v>
       </c>
-      <c r="J10" s="59" t="s">
+      <c r="J10" s="58" t="s">
         <v>913</v>
       </c>
       <c r="K10" s="47"/>
@@ -14016,16 +14027,16 @@
       <c r="C11" s="47"/>
       <c r="D11" s="47"/>
       <c r="E11" s="47"/>
-      <c r="F11" s="59" t="s">
+      <c r="F11" s="58" t="s">
         <v>910</v>
       </c>
-      <c r="G11" s="59" t="s">
+      <c r="G11" s="58" t="s">
         <v>911</v>
       </c>
-      <c r="H11" s="59" t="s">
+      <c r="H11" s="58" t="s">
         <v>912</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="58" t="s">
         <v>913</v>
       </c>
       <c r="J11" s="47"/>
@@ -14048,16 +14059,16 @@
       <c r="D12" s="47" t="s">
         <v>916</v>
       </c>
-      <c r="E12" s="59" t="s">
+      <c r="E12" s="58" t="s">
         <v>910</v>
       </c>
-      <c r="F12" s="59" t="s">
+      <c r="F12" s="58" t="s">
         <v>911</v>
       </c>
-      <c r="G12" s="59" t="s">
+      <c r="G12" s="58" t="s">
         <v>912</v>
       </c>
-      <c r="H12" s="59" t="s">
+      <c r="H12" s="58" t="s">
         <v>913</v>
       </c>
       <c r="I12" s="47"/>
@@ -14078,16 +14089,16 @@
       <c r="C13" s="47" t="s">
         <v>917</v>
       </c>
-      <c r="D13" s="59" t="s">
+      <c r="D13" s="58" t="s">
         <v>910</v>
       </c>
-      <c r="E13" s="59" t="s">
+      <c r="E13" s="58" t="s">
         <v>911</v>
       </c>
-      <c r="F13" s="59" t="s">
+      <c r="F13" s="58" t="s">
         <v>912</v>
       </c>
-      <c r="G13" s="59" t="s">
+      <c r="G13" s="58" t="s">
         <v>913</v>
       </c>
       <c r="H13" s="47"/>
@@ -14106,16 +14117,16 @@
       <c r="B14" s="47" t="s">
         <v>918</v>
       </c>
-      <c r="C14" s="59" t="s">
+      <c r="C14" s="58" t="s">
         <v>910</v>
       </c>
-      <c r="D14" s="59" t="s">
+      <c r="D14" s="58" t="s">
         <v>911</v>
       </c>
-      <c r="E14" s="59" t="s">
+      <c r="E14" s="58" t="s">
         <v>912</v>
       </c>
-      <c r="F14" s="59" t="s">
+      <c r="F14" s="58" t="s">
         <v>913</v>
       </c>
       <c r="G14" s="47"/>
@@ -14132,16 +14143,16 @@
       <c r="A15" s="6">
         <v>50</v>
       </c>
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="58" t="s">
         <v>910</v>
       </c>
-      <c r="C15" s="59" t="s">
+      <c r="C15" s="58" t="s">
         <v>911</v>
       </c>
-      <c r="D15" s="59" t="s">
+      <c r="D15" s="58" t="s">
         <v>912</v>
       </c>
-      <c r="E15" s="59" t="s">
+      <c r="E15" s="58" t="s">
         <v>913</v>
       </c>
       <c r="F15" s="47"/>
@@ -14159,13 +14170,13 @@
       <c r="A16" s="6">
         <v>55</v>
       </c>
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="58" t="s">
         <v>911</v>
       </c>
-      <c r="C16" s="59" t="s">
+      <c r="C16" s="58" t="s">
         <v>912</v>
       </c>
-      <c r="D16" s="59" t="s">
+      <c r="D16" s="58" t="s">
         <v>913</v>
       </c>
       <c r="E16" s="47"/>
@@ -14184,10 +14195,10 @@
       <c r="A17" s="6">
         <v>60</v>
       </c>
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="58" t="s">
         <v>912</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="58" t="s">
         <v>913</v>
       </c>
       <c r="D17" s="47"/>
@@ -14207,7 +14218,7 @@
       <c r="A18" s="6">
         <v>65</v>
       </c>
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="58" t="s">
         <v>913</v>
       </c>
       <c r="C18" s="47"/>
@@ -14224,48 +14235,48 @@
       <c r="N18" s="47"/>
       <c r="O18" s="47"/>
     </row>
-    <row r="19" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>919</v>
       </c>
       <c r="B19" s="47"/>
-      <c r="C19" s="60" t="s">
+      <c r="C19" s="59" t="s">
         <v>918</v>
       </c>
-      <c r="D19" s="60" t="s">
+      <c r="D19" s="59" t="s">
         <v>920</v>
       </c>
-      <c r="E19" s="60" t="s">
+      <c r="E19" s="59" t="s">
         <v>921</v>
       </c>
-      <c r="F19" s="60" t="s">
+      <c r="F19" s="59" t="s">
         <v>921</v>
       </c>
-      <c r="G19" s="60" t="s">
+      <c r="G19" s="59" t="s">
         <v>922</v>
       </c>
-      <c r="H19" s="60" t="s">
+      <c r="H19" s="59" t="s">
         <v>922</v>
       </c>
-      <c r="I19" s="60" t="s">
+      <c r="I19" s="59" t="s">
         <v>922</v>
       </c>
-      <c r="J19" s="60" t="s">
+      <c r="J19" s="59" t="s">
         <v>923</v>
       </c>
-      <c r="K19" s="60" t="s">
+      <c r="K19" s="59" t="s">
         <v>924</v>
       </c>
-      <c r="L19" s="60" t="s">
+      <c r="L19" s="59" t="s">
         <v>925</v>
       </c>
-      <c r="M19" s="60" t="s">
+      <c r="M19" s="59" t="s">
         <v>926</v>
       </c>
-      <c r="N19" s="60" t="s">
+      <c r="N19" s="59" t="s">
         <v>927</v>
       </c>
-      <c r="O19" s="60" t="s">
+      <c r="O19" s="59" t="s">
         <v>928</v>
       </c>
     </row>
@@ -14273,93 +14284,93 @@
       <c r="A20" s="6" t="s">
         <v>876</v>
       </c>
-      <c r="B20" s="61">
+      <c r="B20" s="60">
         <v>43854</v>
       </c>
-      <c r="C20" s="61">
+      <c r="C20" s="60">
         <v>43854</v>
       </c>
-      <c r="D20" s="61">
+      <c r="D20" s="60">
         <v>43854</v>
       </c>
-      <c r="E20" s="61">
+      <c r="E20" s="60">
         <v>43854</v>
       </c>
-      <c r="F20" s="61">
+      <c r="F20" s="60">
         <v>43854</v>
       </c>
-      <c r="G20" s="61">
+      <c r="G20" s="60">
         <v>43854</v>
       </c>
-      <c r="H20" s="61">
+      <c r="H20" s="60">
         <v>43854</v>
       </c>
-      <c r="I20" s="61">
+      <c r="I20" s="60">
         <v>43854</v>
       </c>
-      <c r="J20" s="61">
+      <c r="J20" s="60">
         <v>43854</v>
       </c>
-      <c r="K20" s="61">
+      <c r="K20" s="60">
         <v>43854</v>
       </c>
-      <c r="L20" s="61">
+      <c r="L20" s="60">
         <v>43854</v>
       </c>
-      <c r="M20" s="61">
+      <c r="M20" s="60">
         <v>43854</v>
       </c>
-      <c r="N20" s="61">
+      <c r="N20" s="60">
         <v>43854</v>
       </c>
-      <c r="O20" s="61">
+      <c r="O20" s="60">
         <v>43854</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>850</v>
       </c>
-      <c r="B21" s="59">
+      <c r="B21" s="58">
         <v>0</v>
       </c>
-      <c r="C21" s="59">
+      <c r="C21" s="58">
         <v>0</v>
       </c>
-      <c r="D21" s="59">
+      <c r="D21" s="58">
         <v>0</v>
       </c>
-      <c r="E21" s="59">
+      <c r="E21" s="58">
         <v>0</v>
       </c>
-      <c r="F21" s="59">
+      <c r="F21" s="58">
         <v>0</v>
       </c>
-      <c r="G21" s="59">
+      <c r="G21" s="58">
         <v>0</v>
       </c>
-      <c r="H21" s="59">
+      <c r="H21" s="58">
         <v>0</v>
       </c>
-      <c r="I21" s="59">
+      <c r="I21" s="58">
         <v>0</v>
       </c>
-      <c r="J21" s="59">
+      <c r="J21" s="58">
         <v>0</v>
       </c>
-      <c r="K21" s="59">
+      <c r="K21" s="58">
         <v>0</v>
       </c>
-      <c r="L21" s="59">
+      <c r="L21" s="58">
         <v>0</v>
       </c>
-      <c r="M21" s="59">
+      <c r="M21" s="58">
         <v>0</v>
       </c>
-      <c r="N21" s="59">
+      <c r="N21" s="58">
         <v>0</v>
       </c>
-      <c r="O21" s="59">
+      <c r="O21" s="58">
         <v>0</v>
       </c>
     </row>
@@ -14393,23 +14404,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="67" t="s">
         <v>930</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="70"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="69"/>
     </row>
     <row r="2" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -14428,16 +14439,16 @@
         <v>934</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="67"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="66"/>
     </row>
     <row r="4" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
@@ -14450,7 +14461,7 @@
       <c r="D4" s="47" t="s">
         <v>936</v>
       </c>
-      <c r="E4" s="62" t="s">
+      <c r="E4" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14465,7 +14476,7 @@
       <c r="D5" s="47" t="s">
         <v>939</v>
       </c>
-      <c r="E5" s="62" t="s">
+      <c r="E5" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14480,7 +14491,7 @@
       <c r="D6" s="47" t="s">
         <v>941</v>
       </c>
-      <c r="E6" s="62" t="s">
+      <c r="E6" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14495,7 +14506,7 @@
       <c r="D7" s="47" t="s">
         <v>943</v>
       </c>
-      <c r="E7" s="62" t="s">
+      <c r="E7" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14510,7 +14521,7 @@
       <c r="D8" s="47" t="s">
         <v>945</v>
       </c>
-      <c r="E8" s="62" t="s">
+      <c r="E8" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14525,7 +14536,7 @@
       <c r="D9" s="47" t="s">
         <v>947</v>
       </c>
-      <c r="E9" s="62" t="s">
+      <c r="E9" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14542,7 +14553,7 @@
       <c r="D10" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E10" s="62" t="s">
+      <c r="E10" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14559,7 +14570,7 @@
       <c r="D11" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E11" s="62" t="s">
+      <c r="E11" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14576,7 +14587,7 @@
       <c r="D12" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E12" s="62" t="s">
+      <c r="E12" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14593,7 +14604,7 @@
       <c r="D13" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E13" s="62" t="s">
+      <c r="E13" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14610,7 +14621,7 @@
       <c r="D14" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E14" s="62" t="s">
+      <c r="E14" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14627,7 +14638,7 @@
       <c r="D15" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E15" s="62" t="s">
+      <c r="E15" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14644,7 +14655,7 @@
       <c r="D16" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E16" s="62" t="s">
+      <c r="E16" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14661,7 +14672,7 @@
       <c r="D17" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E17" s="62" t="s">
+      <c r="E17" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14678,7 +14689,7 @@
       <c r="D18" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E18" s="62" t="s">
+      <c r="E18" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14695,7 +14706,7 @@
       <c r="D19" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E19" s="62" t="s">
+      <c r="E19" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14712,7 +14723,7 @@
       <c r="D20" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E20" s="62" t="s">
+      <c r="E20" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14729,7 +14740,7 @@
       <c r="D21" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E21" s="62" t="s">
+      <c r="E21" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14746,7 +14757,7 @@
       <c r="D22" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E22" s="62" t="s">
+      <c r="E22" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14763,7 +14774,7 @@
       <c r="D23" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E23" s="62" t="s">
+      <c r="E23" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14780,7 +14791,7 @@
       <c r="D24" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E24" s="62" t="s">
+      <c r="E24" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14797,7 +14808,7 @@
       <c r="D25" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E25" s="62" t="s">
+      <c r="E25" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14814,7 +14825,7 @@
       <c r="D26" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E26" s="62" t="s">
+      <c r="E26" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14831,7 +14842,7 @@
       <c r="D27" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E27" s="62" t="s">
+      <c r="E27" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14848,7 +14859,7 @@
       <c r="D28" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E28" s="62" t="s">
+      <c r="E28" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14865,7 +14876,7 @@
       <c r="D29" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E29" s="62" t="s">
+      <c r="E29" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14882,7 +14893,7 @@
       <c r="D30" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E30" s="62" t="s">
+      <c r="E30" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14899,7 +14910,7 @@
       <c r="D31" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E31" s="62" t="s">
+      <c r="E31" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14916,7 +14927,7 @@
       <c r="D32" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E32" s="62" t="s">
+      <c r="E32" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14933,7 +14944,7 @@
       <c r="D33" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E33" s="62" t="s">
+      <c r="E33" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14950,7 +14961,7 @@
       <c r="D34" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E34" s="62" t="s">
+      <c r="E34" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14967,7 +14978,7 @@
       <c r="D35" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E35" s="62" t="s">
+      <c r="E35" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -14984,7 +14995,7 @@
       <c r="D36" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E36" s="62" t="s">
+      <c r="E36" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -15001,7 +15012,7 @@
       <c r="D37" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E37" s="62" t="s">
+      <c r="E37" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -15018,7 +15029,7 @@
       <c r="D38" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E38" s="62" t="s">
+      <c r="E38" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -15035,7 +15046,7 @@
       <c r="D39" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E39" s="62" t="s">
+      <c r="E39" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -15052,7 +15063,7 @@
       <c r="D40" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E40" s="62" t="s">
+      <c r="E40" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -15069,7 +15080,7 @@
       <c r="D41" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E41" s="62" t="s">
+      <c r="E41" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -15086,7 +15097,7 @@
       <c r="D42" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E42" s="62" t="s">
+      <c r="E42" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -15103,7 +15114,7 @@
       <c r="D43" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E43" s="62" t="s">
+      <c r="E43" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -15120,7 +15131,7 @@
       <c r="D44" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E44" s="62" t="s">
+      <c r="E44" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -15128,7 +15139,7 @@
       <c r="A45" s="46">
         <v>58</v>
       </c>
-      <c r="B45" s="63" t="s">
+      <c r="B45" s="62" t="s">
         <v>1019</v>
       </c>
       <c r="C45" s="47" t="s">
@@ -15137,7 +15148,7 @@
       <c r="D45" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E45" s="62" t="s">
+      <c r="E45" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -15145,7 +15156,7 @@
       <c r="A46" s="46">
         <v>59</v>
       </c>
-      <c r="B46" s="63" t="s">
+      <c r="B46" s="62" t="s">
         <v>1021</v>
       </c>
       <c r="C46" s="47" t="s">
@@ -15154,7 +15165,7 @@
       <c r="D46" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E46" s="62" t="s">
+      <c r="E46" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -15162,7 +15173,7 @@
       <c r="A47" s="46">
         <v>60</v>
       </c>
-      <c r="B47" s="63" t="s">
+      <c r="B47" s="62" t="s">
         <v>1023</v>
       </c>
       <c r="C47" s="47" t="s">
@@ -15171,7 +15182,7 @@
       <c r="D47" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E47" s="62" t="s">
+      <c r="E47" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -15179,7 +15190,7 @@
       <c r="A48" s="46">
         <v>61</v>
       </c>
-      <c r="B48" s="63" t="s">
+      <c r="B48" s="62" t="s">
         <v>1025</v>
       </c>
       <c r="C48" s="47" t="s">
@@ -15188,7 +15199,7 @@
       <c r="D48" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E48" s="62" t="s">
+      <c r="E48" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -15196,7 +15207,7 @@
       <c r="A49" s="46">
         <v>62</v>
       </c>
-      <c r="B49" s="63" t="s">
+      <c r="B49" s="62" t="s">
         <v>1027</v>
       </c>
       <c r="C49" s="47" t="s">
@@ -15205,7 +15216,7 @@
       <c r="D49" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E49" s="62" t="s">
+      <c r="E49" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -15213,7 +15224,7 @@
       <c r="A50" s="46">
         <v>63</v>
       </c>
-      <c r="B50" s="63" t="s">
+      <c r="B50" s="62" t="s">
         <v>1029</v>
       </c>
       <c r="C50" s="47" t="s">
@@ -15222,7 +15233,7 @@
       <c r="D50" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E50" s="62" t="s">
+      <c r="E50" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -15230,7 +15241,7 @@
       <c r="A51" s="46">
         <v>64</v>
       </c>
-      <c r="B51" s="63" t="s">
+      <c r="B51" s="62" t="s">
         <v>1031</v>
       </c>
       <c r="C51" s="47" t="s">
@@ -15239,7 +15250,7 @@
       <c r="D51" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E51" s="62" t="s">
+      <c r="E51" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -15247,7 +15258,7 @@
       <c r="A52" s="46">
         <v>65</v>
       </c>
-      <c r="B52" s="63">
+      <c r="B52" s="62">
         <v>0</v>
       </c>
       <c r="C52" s="47" t="s">
@@ -15256,7 +15267,7 @@
       <c r="D52" s="47" t="s">
         <v>950</v>
       </c>
-      <c r="E52" s="62" t="s">
+      <c r="E52" s="61" t="s">
         <v>937</v>
       </c>
     </row>
@@ -15271,7 +15282,7 @@
       <c r="D53" s="30">
         <v>5</v>
       </c>
-      <c r="E53" s="64">
+      <c r="E53" s="63">
         <v>13</v>
       </c>
     </row>

</xml_diff>